<commit_message>
ESS cost data. 2025 and 2035
</commit_message>
<xml_diff>
--- a/data/IEEE9/Shared ESS/ieee9_ESS.xlsx
+++ b/data/IEEE9/Shared ESS/ieee9_ESS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\IEEE_9\Shared ESS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\IEEE9\Shared ESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B41C1E-1D85-4835-B836-F25E13DA9994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D282252B-647B-4AD3-9E96-91388492104C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="3840" windowWidth="21600" windowHeight="12660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="81" r:id="rId1"/>
@@ -74,12 +74,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -94,10 +100,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,7 +387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E7A88E-2477-46FD-BE5E-2BB647C1CD4A}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -416,7 +423,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,33 +506,43 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2823AF14-4748-4019-BD7D-F91F970D3C5E}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>2020</v>
       </c>
       <c r="C1">
+        <v>2025</v>
+      </c>
+      <c r="D1">
         <v>2030</v>
       </c>
-      <c r="D1">
+      <c r="E1">
+        <v>2035</v>
+      </c>
+      <c r="F1">
         <v>2040</v>
       </c>
-      <c r="E1">
+      <c r="G1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -533,20 +550,28 @@
         <f>(1/5)*'Investment Cost NREL'!B3*1000</f>
         <v>69000</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
+        <f>AVERAGE(D2,B2)</f>
+        <v>54300</v>
+      </c>
+      <c r="D2" s="2">
         <f>(1/5)*'Investment Cost NREL'!C3*1000</f>
         <v>39600</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="3">
+        <f>AVERAGE(F2,D2)</f>
+        <v>37200</v>
+      </c>
+      <c r="F2" s="2">
         <f>(1/5)*'Investment Cost NREL'!D3*1000</f>
         <v>34800.000000000007</v>
       </c>
-      <c r="E2" s="2">
+      <c r="G2" s="2">
         <f>(1/5)*'Investment Cost NREL'!E3*1000</f>
         <v>29800</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -554,15 +579,23 @@
         <f>(4/5)*'Investment Cost NREL'!B3*1000</f>
         <v>276000</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
+        <f>AVERAGE(D3,B3)</f>
+        <v>217200</v>
+      </c>
+      <c r="D3" s="2">
         <f>(4/5)*'Investment Cost NREL'!C3*1000</f>
         <v>158400</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="3">
+        <f>AVERAGE(F3,D3)</f>
+        <v>148800</v>
+      </c>
+      <c r="F3" s="2">
         <f>(4/5)*'Investment Cost NREL'!D3*1000</f>
         <v>139200.00000000003</v>
       </c>
-      <c r="E3" s="2">
+      <c r="G3" s="2">
         <f>(4/5)*'Investment Cost NREL'!E3*1000</f>
         <v>119200</v>
       </c>

</xml_diff>

<commit_message>
TN. Years 2040-2055 added.
</commit_message>
<xml_diff>
--- a/data/IEEE9/Shared ESS/ieee9_ESS.xlsx
+++ b/data/IEEE9/Shared ESS/ieee9_ESS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\IEEE9\Shared ESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C77D9A-8F53-4966-97BD-CD83EF8F2A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042377F2-D5D1-4B25-9B16-90696D870F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -995,7 +995,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2823AF14-4748-4019-BD7D-F91F970D3C5E}">
   <dimension ref="A1:AK3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AH2" sqref="AH2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1115,16 +1117,16 @@
         <v>2051</v>
       </c>
       <c r="AH1" s="4">
-        <v>2050</v>
+        <v>2052</v>
       </c>
       <c r="AI1" s="4">
-        <v>2050</v>
+        <v>2053</v>
       </c>
       <c r="AJ1" s="4">
-        <v>2050</v>
+        <v>2054</v>
       </c>
       <c r="AK1" s="4">
-        <v>2050</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>